<commit_message>
Feat(index.html): fazendo responsividade da primeira seção da home-page
</commit_message>
<xml_diff>
--- a/Documentação/TotemHub - Backlog.xlsx
+++ b/Documentação/TotemHub - Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bandtec_TotemHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\Git\Bandtec_TotemHub\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670036AE-2118-4EBD-8F20-39B1752DC284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7C5557-3420-433A-8D4E-27F0ACA12875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Lista de reqs." sheetId="3" r:id="rId1"/>
     <sheet name="Refatoração Estrutura" sheetId="4" r:id="rId2"/>
     <sheet name="User Story" sheetId="5" r:id="rId3"/>
-    <sheet name="Planilha2" sheetId="6" r:id="rId4"/>
+    <sheet name="Lean UX" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Lista de reqs.'!$G$4:$I$4</definedName>
@@ -637,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -675,6 +675,126 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -684,146 +804,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -886,6 +875,18 @@
           <color theme="3" tint="-0.249977111117893"/>
         </right>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1022,16 +1023,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9AD0C298-A3C4-4B6D-A826-3F4FDA3611BC}" name="Tabela2" displayName="Tabela2" ref="C4:I22" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9AD0C298-A3C4-4B6D-A826-3F4FDA3611BC}" name="Tabela2" displayName="Tabela2" ref="C4:I22" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="C4:I22" xr:uid="{E4E6A3FB-FD8D-435E-AFC5-2349C9D21F73}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{97D85B41-9860-4CD6-B68A-0F415CA5CC92}" name="Estado" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{53156FB0-92E5-4B86-BE2B-46C7F61C34DC}" name="Artefato de referência" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{FB97AF01-D5F2-4F8A-86F7-BCD92C00AE2F}" name="Requisito" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{AB0A7A6A-87D8-4F19-BC58-69B293139831}" name="Descrição do requisito" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{0A12B184-8A4D-426F-9E70-E9503B1100F2}" name="Essencial" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{B79ECEB9-B207-4E45-873B-790E6DCAEC3A}" name="Importante" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{B0EE7D0E-8FE0-42D4-83DE-B48C430B7A72}" name="Desejavel" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{97D85B41-9860-4CD6-B68A-0F415CA5CC92}" name="Estado" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{53156FB0-92E5-4B86-BE2B-46C7F61C34DC}" name="Artefato de referência" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{FB97AF01-D5F2-4F8A-86F7-BCD92C00AE2F}" name="Requisito" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{AB0A7A6A-87D8-4F19-BC58-69B293139831}" name="Descrição do requisito" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{0A12B184-8A4D-426F-9E70-E9503B1100F2}" name="Essencial" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{B79ECEB9-B207-4E45-873B-790E6DCAEC3A}" name="Importante" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{B0EE7D0E-8FE0-42D4-83DE-B48C430B7A72}" name="Desejavel" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1376,12 +1377,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="7:23" s="18" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="7:23" ht="31.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="G2" s="21" t="s">
+    <row r="2" spans="7:23" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="G2" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="63"/>
       <c r="W2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1651,499 +1652,499 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D365EA23-5304-45D0-B9B5-2768DD50B9BF}">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.625" style="15"/>
-    <col min="3" max="3" width="13.625" style="57" customWidth="1"/>
-    <col min="4" max="4" width="24.125" style="57" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.125" style="57" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.25" style="57" customWidth="1"/>
-    <col min="7" max="7" width="13.625" style="57" customWidth="1"/>
-    <col min="8" max="8" width="14.375" style="57" customWidth="1"/>
-    <col min="9" max="9" width="13.375" style="57" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="53" customWidth="1"/>
+    <col min="4" max="4" width="24.125" style="53" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.125" style="53" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.25" style="53" customWidth="1"/>
+    <col min="7" max="7" width="13.625" style="53" customWidth="1"/>
+    <col min="8" max="8" width="14.375" style="53" customWidth="1"/>
+    <col min="9" max="9" width="13.375" style="53" customWidth="1"/>
     <col min="10" max="18" width="8.625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-    </row>
-    <row r="2" spans="2:9" s="15" customFormat="1" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="26" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+    </row>
+    <row r="2" spans="2:9" s="15" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="2:9" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="16"/>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="23" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="16"/>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="33"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="29"/>
     </row>
     <row r="6" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="16"/>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="37"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="33"/>
     </row>
     <row r="7" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="17"/>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="39"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="35"/>
     </row>
     <row r="8" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="16"/>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="41"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="37"/>
     </row>
     <row r="9" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="16"/>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="39"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="35"/>
     </row>
     <row r="10" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="16"/>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="44" t="s">
+      <c r="F10" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="41"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="37"/>
     </row>
     <row r="11" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="16"/>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="46" t="s">
+      <c r="F11" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="39"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="35"/>
     </row>
     <row r="12" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="16"/>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="41"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="37"/>
     </row>
     <row r="13" spans="2:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="16"/>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="46" t="s">
+      <c r="F13" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="31"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="47"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="43"/>
     </row>
     <row r="14" spans="2:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="16"/>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="50" t="s">
+      <c r="E14" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="51" t="s">
+      <c r="F14" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="31"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="52"/>
-    </row>
-    <row r="15" spans="2:9" s="24" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="58" t="s">
+      <c r="G14" s="27"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="48"/>
+    </row>
+    <row r="15" spans="2:9" s="21" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="59" t="s">
+      <c r="D15" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="59" t="s">
+      <c r="E15" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="59" t="s">
+      <c r="F15" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="60"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="61"/>
-    </row>
-    <row r="16" spans="2:9" s="24" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="63" t="s">
+      <c r="G15" s="56"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="57"/>
+    </row>
+    <row r="16" spans="2:9" s="21" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="44" t="s">
+      <c r="E16" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="62" t="s">
+      <c r="F16" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="60"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="64"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="60"/>
     </row>
     <row r="17" spans="3:9" s="15" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="38" t="s">
+      <c r="E17" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="43" t="s">
+      <c r="F17" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="39"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="35"/>
     </row>
     <row r="18" spans="3:9" s="15" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="44" t="s">
+      <c r="F18" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="41"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="37"/>
     </row>
     <row r="19" spans="3:9" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="35" t="s">
+      <c r="F19" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="G19" s="53"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="41"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="37"/>
     </row>
     <row r="20" spans="3:9" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="35" t="s">
+      <c r="E20" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="53"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="41"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="37"/>
     </row>
     <row r="21" spans="3:9" s="15" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="35" t="s">
+      <c r="E21" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="G21" s="53"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="41"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="37"/>
     </row>
     <row r="22" spans="3:9" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="35" t="s">
+      <c r="E22" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="35" t="s">
+      <c r="F22" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="G22" s="53"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="55"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="51"/>
     </row>
     <row r="23" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
     </row>
     <row r="24" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="56"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
     </row>
     <row r="25" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
     </row>
     <row r="26" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="56"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
     </row>
     <row r="27" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="56"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
     </row>
     <row r="28" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="56"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
     </row>
     <row r="29" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="56"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
     </row>
     <row r="30" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
     </row>
     <row r="31" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
     </row>
     <row r="32" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
     </row>
     <row r="33" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="56"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="52"/>
     </row>
     <row r="34" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="56"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2172,14 +2173,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECFABF79-7CBD-4857-A8FB-1108C995F101}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="21" width="9" style="65"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="65" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
alterando documentacao e backlog
</commit_message>
<xml_diff>
--- a/Documentação/TotemHub - Backlog.xlsx
+++ b/Documentação/TotemHub - Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bandtec_TotemHub\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CE29B6-3FC8-4A7C-AE33-0A8EBA38ED47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8813915-8FF8-4148-A256-064E7BC592CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="77">
   <si>
     <t>Essencial</t>
   </si>
@@ -245,6 +245,18 @@
   </si>
   <si>
     <t>Entrar em Contato</t>
+  </si>
+  <si>
+    <t>Controle de versionamento via Github</t>
+  </si>
+  <si>
+    <t>Utilização de github para versionamento e desenvolvimento do projeto</t>
+  </si>
+  <si>
+    <t>Documentação atualizada</t>
+  </si>
+  <si>
+    <t>Atualização da documentação com base nas informações adquiridas ao longo da sprint2.</t>
   </si>
 </sst>
 </file>
@@ -358,7 +370,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -724,11 +736,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -883,6 +908,36 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -895,34 +950,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1073,15 +1107,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>272498</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>97734</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>295952</xdr:colOff>
+      <xdr:colOff>320800</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>190985</xdr:rowOff>
+      <xdr:rowOff>174419</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1104,8 +1138,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9163050" y="514350"/>
-          <a:ext cx="4848902" cy="3477110"/>
+          <a:off x="9209433" y="495299"/>
+          <a:ext cx="4860497" cy="3455990"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1184,8 +1218,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9AD0C298-A3C4-4B6D-A826-3F4FDA3611BC}" name="Tabela2" displayName="Tabela2" ref="C4:I27" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="C4:I27" xr:uid="{E4E6A3FB-FD8D-435E-AFC5-2349C9D21F73}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9AD0C298-A3C4-4B6D-A826-3F4FDA3611BC}" name="Tabela2" displayName="Tabela2" ref="C4:I29" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="C4:I29" xr:uid="{E4E6A3FB-FD8D-435E-AFC5-2349C9D21F73}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{97D85B41-9860-4CD6-B68A-0F415CA5CC92}" name="Estado" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{53156FB0-92E5-4B86-BE2B-46C7F61C34DC}" name="Artefato de referência" dataDxfId="5"/>
@@ -1523,7 +1557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{746770E9-57AE-43AC-96BA-C5185126D1A5}">
   <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -1539,11 +1573,11 @@
   <sheetData>
     <row r="1" spans="7:23" s="18" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="7:23" ht="31.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="72"/>
       <c r="W2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1813,8 +1847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D365EA23-5304-45D0-B9B5-2768DD50B9BF}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView showGridLines="0" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1840,15 +1874,15 @@
       <c r="I1" s="22"/>
     </row>
     <row r="2" spans="2:9" s="15" customFormat="1" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
     </row>
     <row r="3" spans="2:9" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="22"/>
@@ -2189,108 +2223,116 @@
       <c r="D22" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="64" t="s">
+      <c r="E22" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="64" t="s">
+      <c r="F22" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="65"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="68"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="64"/>
     </row>
     <row r="23" spans="3:9" s="15" customFormat="1" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="66" t="s">
+      <c r="C23" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="67"/>
-      <c r="E23" s="69" t="s">
+      <c r="D23" s="63"/>
+      <c r="E23" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="F23" s="69" t="s">
+      <c r="F23" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="G23" s="70"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="69"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="65"/>
     </row>
     <row r="24" spans="3:9" s="15" customFormat="1" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="66" t="s">
+      <c r="C24" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="67"/>
-      <c r="E24" s="69" t="s">
+      <c r="D24" s="63"/>
+      <c r="E24" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="F24" s="71" t="s">
+      <c r="F24" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="G24" s="70"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="69"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
     </row>
     <row r="25" spans="3:9" s="15" customFormat="1" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="66" t="s">
+      <c r="C25" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="67"/>
-      <c r="E25" s="69" t="s">
+      <c r="D25" s="63"/>
+      <c r="E25" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="F25" s="71" t="s">
+      <c r="F25" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="G25" s="70"/>
-      <c r="H25" s="69"/>
-      <c r="I25" s="69"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="65"/>
     </row>
     <row r="26" spans="3:9" s="15" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="66" t="s">
+      <c r="C26" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="67"/>
-      <c r="E26" s="69" t="s">
+      <c r="D26" s="63"/>
+      <c r="E26" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="F26" s="71" t="s">
+      <c r="F26" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="G26" s="70"/>
-      <c r="H26" s="69"/>
-      <c r="I26" s="72"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="68"/>
     </row>
     <row r="27" spans="3:9" s="15" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="66" t="s">
+      <c r="C27" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="67"/>
-      <c r="E27" s="69" t="s">
+      <c r="D27" s="63"/>
+      <c r="E27" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="F27" s="71" t="s">
+      <c r="F27" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="G27" s="69"/>
-      <c r="H27" s="73"/>
-      <c r="I27" s="69"/>
-    </row>
-    <row r="28" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="51"/>
-    </row>
-    <row r="29" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="69"/>
+      <c r="I27" s="65"/>
+    </row>
+    <row r="28" spans="3:9" s="15" customFormat="1" ht="41.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="62"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" s="75" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="66"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="74"/>
+    </row>
+    <row r="29" spans="3:9" s="15" customFormat="1" ht="41.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="62"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="G29" s="76"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="74"/>
     </row>
     <row r="30" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="51"/>
@@ -2335,8 +2377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288FC3E7-48B0-4EA1-84BD-030D133D4615}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
atualizando documentação e backlog do projeto
</commit_message>
<xml_diff>
--- a/Documentação/TotemHub - Backlog.xlsx
+++ b/Documentação/TotemHub - Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bandtec_TotemHub\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8813915-8FF8-4148-A256-064E7BC592CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2FB174-A4AB-4231-A7E2-3989F321467E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de reqs." sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="84">
   <si>
     <t>Essencial</t>
   </si>
@@ -199,9 +199,6 @@
     <t>Desgin intuitivo para navegação fluída do site</t>
   </si>
   <si>
-    <t>Controle de permissão para segurança do site</t>
-  </si>
-  <si>
     <t>Dashboard Intuitiva</t>
   </si>
   <si>
@@ -214,9 +211,6 @@
     <t>Feedback via QRCode</t>
   </si>
   <si>
-    <t>API de consulta dos dados de máquina no BD (looca)</t>
-  </si>
-  <si>
     <t>API para consulta dos dados de máquina do totem</t>
   </si>
   <si>
@@ -257,13 +251,40 @@
   </si>
   <si>
     <t>Atualização da documentação com base nas informações adquiridas ao longo da sprint2.</t>
+  </si>
+  <si>
+    <t>Validação de informações baseadas no BD</t>
+  </si>
+  <si>
+    <t>Monitoramento do SO (totem)</t>
+  </si>
+  <si>
+    <t>Validação de sessões e logof de usuário</t>
+  </si>
+  <si>
+    <t>Integração captando dados de máquina</t>
+  </si>
+  <si>
+    <t>Padronização de elementos</t>
+  </si>
+  <si>
+    <t>Padronização de todos os elementos de interação dos usuários da aplicação</t>
+  </si>
+  <si>
+    <t>Controle de permissão com base em adicionar e retirar usuários cadastrados na aplicação</t>
+  </si>
+  <si>
+    <t>UX#006</t>
+  </si>
+  <si>
+    <t>Validação de sessão de usuário baseado no login que está acessando a aplicação</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -303,6 +324,22 @@
     <font>
       <sz val="12"/>
       <color theme="8" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -370,7 +407,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -445,26 +482,6 @@
       </top>
       <bottom style="medium">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
       </bottom>
       <diagonal/>
     </border>
@@ -490,189 +507,8 @@
       <right style="medium">
         <color theme="3" tint="-0.249977111117893"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </right>
-      <top style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </left>
-      <right style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </left>
-      <right style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </left>
-      <right style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </right>
-      <top style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </left>
-      <right style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color theme="3" tint="-0.249977111117893"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -711,10 +547,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color theme="3" tint="-0.249977111117893"/>
       </left>
-      <right style="medium">
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -728,22 +586,18 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -753,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -797,173 +651,118 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1028,15 +827,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -1218,16 +1008,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9AD0C298-A3C4-4B6D-A826-3F4FDA3611BC}" name="Tabela2" displayName="Tabela2" ref="C4:I29" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="C4:I29" xr:uid="{E4E6A3FB-FD8D-435E-AFC5-2349C9D21F73}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9AD0C298-A3C4-4B6D-A826-3F4FDA3611BC}" name="Tabela2" displayName="Tabela2" ref="C4:I31" totalsRowShown="0" headerRowDxfId="0" dataDxfId="8">
+  <autoFilter ref="C4:I31" xr:uid="{E4E6A3FB-FD8D-435E-AFC5-2349C9D21F73}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{97D85B41-9860-4CD6-B68A-0F415CA5CC92}" name="Estado" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{53156FB0-92E5-4B86-BE2B-46C7F61C34DC}" name="Artefato de referência" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{FB97AF01-D5F2-4F8A-86F7-BCD92C00AE2F}" name="Requisito" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{AB0A7A6A-87D8-4F19-BC58-69B293139831}" name="Descrição do requisito" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{0A12B184-8A4D-426F-9E70-E9503B1100F2}" name="Essencial" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{B79ECEB9-B207-4E45-873B-790E6DCAEC3A}" name="Importante" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{B0EE7D0E-8FE0-42D4-83DE-B48C430B7A72}" name="Desejavel" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{97D85B41-9860-4CD6-B68A-0F415CA5CC92}" name="Estado" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{53156FB0-92E5-4B86-BE2B-46C7F61C34DC}" name="Artefato de referência" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{FB97AF01-D5F2-4F8A-86F7-BCD92C00AE2F}" name="Requisito" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{AB0A7A6A-87D8-4F19-BC58-69B293139831}" name="Descrição do requisito" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{0A12B184-8A4D-426F-9E70-E9503B1100F2}" name="Essencial" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{B79ECEB9-B207-4E45-873B-790E6DCAEC3A}" name="Importante" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{B0EE7D0E-8FE0-42D4-83DE-B48C430B7A72}" name="Desejavel" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1573,11 +1363,11 @@
   <sheetData>
     <row r="1" spans="7:23" s="18" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="7:23" ht="31.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="G2" s="70" t="s">
+      <c r="G2" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="71"/>
-      <c r="I2" s="72"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="35"/>
       <c r="W2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1721,7 +1511,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="7:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="7:23" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G15" s="7" t="s">
         <v>0</v>
       </c>
@@ -1845,26 +1635,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D365EA23-5304-45D0-B9B5-2768DD50B9BF}">
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="17" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.625" style="15"/>
-    <col min="3" max="3" width="13.625" style="52" customWidth="1"/>
-    <col min="4" max="4" width="24.125" style="52" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.125" style="52" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.25" style="52" customWidth="1"/>
-    <col min="7" max="7" width="13.625" style="52" customWidth="1"/>
-    <col min="8" max="8" width="14.375" style="52" customWidth="1"/>
-    <col min="9" max="9" width="13.375" style="52" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="24.125" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.125" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.25" style="25" customWidth="1"/>
+    <col min="7" max="7" width="13.625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="14.375" style="25" customWidth="1"/>
+    <col min="9" max="9" width="13.375" style="25" customWidth="1"/>
     <col min="10" max="18" width="8.625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -1873,18 +1663,18 @@
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
     </row>
-    <row r="2" spans="2:9" s="15" customFormat="1" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="73" t="s">
+    <row r="2" spans="2:20" s="15" customFormat="1" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-    </row>
-    <row r="3" spans="2:9" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+    </row>
+    <row r="3" spans="2:20" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -1892,474 +1682,519 @@
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
       <c r="I3" s="22"/>
-    </row>
-    <row r="4" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T3" s="51"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="16"/>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="49" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="16"/>
-      <c r="C5" s="25" t="s">
+    <row r="5" spans="2:20" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="29"/>
-    </row>
-    <row r="6" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="16"/>
-      <c r="C6" s="30" t="s">
+      <c r="G5" s="43"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+    </row>
+    <row r="6" spans="2:20" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
+      <c r="C6" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="33"/>
-    </row>
-    <row r="7" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="43"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+    </row>
+    <row r="7" spans="2:20" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="17"/>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="27"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="35"/>
-    </row>
-    <row r="8" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="16"/>
-      <c r="C8" s="36" t="s">
+      <c r="G7" s="43"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+    </row>
+    <row r="8" spans="2:20" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="17"/>
+      <c r="C8" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="37"/>
-    </row>
-    <row r="9" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="16"/>
-      <c r="C9" s="38" t="s">
+      <c r="G8" s="43"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+    </row>
+    <row r="9" spans="2:20" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="17"/>
+      <c r="C9" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="35"/>
-    </row>
-    <row r="10" spans="2:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="16"/>
-      <c r="C10" s="36" t="s">
+      <c r="G9" s="43"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+    </row>
+    <row r="10" spans="2:20" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="17"/>
+      <c r="C10" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="27"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="37"/>
-    </row>
-    <row r="11" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="16"/>
-      <c r="C11" s="41" t="s">
+      <c r="G10" s="43"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" spans="2:20" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="17"/>
+      <c r="C11" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="43"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+    </row>
+    <row r="12" spans="2:20" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="17"/>
+      <c r="C12" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="43"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+    </row>
+    <row r="13" spans="2:20" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="17"/>
+      <c r="C13" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="43"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+    </row>
+    <row r="14" spans="2:20" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="17"/>
+      <c r="C14" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="43"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+    </row>
+    <row r="15" spans="2:20" s="21" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="45"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+    </row>
+    <row r="16" spans="2:20" s="21" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="45"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+    </row>
+    <row r="17" spans="3:9" s="15" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="43"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+    </row>
+    <row r="18" spans="3:9" s="15" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="43"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+    </row>
+    <row r="19" spans="3:9" s="15" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="42"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="42"/>
+    </row>
+    <row r="20" spans="3:9" s="15" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="27"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="27"/>
+    </row>
+    <row r="21" spans="3:9" s="15" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="42"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="42"/>
+    </row>
+    <row r="22" spans="3:9" s="15" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="37"/>
+    </row>
+    <row r="23" spans="3:9" s="15" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="37"/>
+    </row>
+    <row r="24" spans="3:9" s="15" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="43"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+    </row>
+    <row r="25" spans="3:9" s="15" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="43"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+    </row>
+    <row r="26" spans="3:9" s="15" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" s="43"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+    </row>
+    <row r="27" spans="3:9" s="15" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="43"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="50"/>
+    </row>
+    <row r="28" spans="3:9" s="15" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F28" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" s="43"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="47"/>
+    </row>
+    <row r="29" spans="3:9" s="15" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="42"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="42"/>
+    </row>
+    <row r="30" spans="3:9" s="15" customFormat="1" ht="41.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="23"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="27"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="35"/>
-    </row>
-    <row r="12" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="16"/>
-      <c r="C12" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="27"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="37"/>
-    </row>
-    <row r="13" spans="2:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="16"/>
-      <c r="C13" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="43"/>
-    </row>
-    <row r="14" spans="2:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="16"/>
-      <c r="C14" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="27"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="48"/>
-    </row>
-    <row r="15" spans="2:9" s="21" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="55"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="56"/>
-    </row>
-    <row r="16" spans="2:9" s="21" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="55"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="59"/>
-    </row>
-    <row r="17" spans="3:9" s="15" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="27"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="35"/>
-    </row>
-    <row r="18" spans="3:9" s="15" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18" s="27"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="37"/>
-    </row>
-    <row r="19" spans="3:9" s="15" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="49"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="37"/>
-    </row>
-    <row r="20" spans="3:9" s="15" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="49"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="37"/>
-    </row>
-    <row r="21" spans="3:9" s="15" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" s="49"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="37"/>
-    </row>
-    <row r="22" spans="3:9" s="15" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22" s="60" t="s">
-        <v>60</v>
-      </c>
-      <c r="G22" s="61"/>
-      <c r="H22" s="60"/>
-      <c r="I22" s="64"/>
-    </row>
-    <row r="23" spans="3:9" s="15" customFormat="1" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="62" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="63"/>
-      <c r="E23" s="65" t="s">
-        <v>62</v>
-      </c>
-      <c r="F23" s="65" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="66"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="65"/>
-    </row>
-    <row r="24" spans="3:9" s="15" customFormat="1" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="63"/>
-      <c r="E24" s="65" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" s="66"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65"/>
-    </row>
-    <row r="25" spans="3:9" s="15" customFormat="1" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="62" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="63"/>
-      <c r="E25" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="G25" s="66"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="65"/>
-    </row>
-    <row r="26" spans="3:9" s="15" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="62" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="63"/>
-      <c r="E26" s="65" t="s">
-        <v>68</v>
-      </c>
-      <c r="F26" s="67" t="s">
-        <v>69</v>
-      </c>
-      <c r="G26" s="66"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="68"/>
-    </row>
-    <row r="27" spans="3:9" s="15" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="62" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="63"/>
-      <c r="E27" s="65" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27" s="67" t="s">
-        <v>71</v>
-      </c>
-      <c r="G27" s="65"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="65"/>
-    </row>
-    <row r="28" spans="3:9" s="15" customFormat="1" ht="41.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="62"/>
-      <c r="D28" s="63"/>
-      <c r="E28" s="60" t="s">
+      <c r="G30" s="41"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+    </row>
+    <row r="31" spans="3:9" s="15" customFormat="1" ht="41.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="28"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="F28" s="75" t="s">
+      <c r="F31" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="G28" s="66"/>
-      <c r="H28" s="74"/>
-      <c r="I28" s="74"/>
-    </row>
-    <row r="29" spans="3:9" s="15" customFormat="1" ht="41.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="62"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="60" t="s">
-        <v>75</v>
-      </c>
-      <c r="F29" s="75" t="s">
-        <v>76</v>
-      </c>
-      <c r="G29" s="76"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="74"/>
-    </row>
-    <row r="30" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-    </row>
-    <row r="31" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="30"/>
     </row>
     <row r="32" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="51"/>
-      <c r="H32" s="51"/>
-      <c r="I32" s="51"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+    </row>
+    <row r="33" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+    </row>
+    <row r="34" spans="3:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2377,7 +2212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288FC3E7-48B0-4EA1-84BD-030D133D4615}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="C8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>

</xml_diff>